<commit_message>
Enhance income-expense type management and user role selection interface
- Added a new "Gider Grubu" section in the income-expense type management page for better categorization.
- Improved the user role selection modal in the sign-in process with enhanced UI and functionality.
- Refactored JavaScript for better readability and maintainability in the role selection modal.
- Updated CSS styles for a more modern look and feel across various components.
- Ensured consistent handling of user input and improved error handling in the role selection process.
</commit_message>
<xml_diff>
--- a/files/kisi_yukleme_sablon.xlsx
+++ b/files/kisi_yukleme_sablon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yonapp-1\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B11810E-53A5-4CA1-9528-564E369C83CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03124B0-BA99-42EB-961A-DA101DE22C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>HP</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{F4F1FEC8-30E0-4F41-9590-76E964C40D14}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{F4F1FEC8-30E0-4F41-9590-76E964C40D14}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{FA5A5C9C-DB28-4ED9-B499-9CCFC4D98835}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{FA5A5C9C-DB28-4ED9-B499-9CCFC4D98835}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{74AB5615-7FC9-4CBB-B957-F67DB61C99AF}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{74AB5615-7FC9-4CBB-B957-F67DB61C99AF}">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{01F7D313-5B87-447E-9486-8C4439387927}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{01F7D313-5B87-447E-9486-8C4439387927}">
       <text>
         <r>
           <rPr>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Sıra</t>
   </si>
@@ -191,31 +191,37 @@
     <t>Daire Tipi*</t>
   </si>
   <si>
-    <t>ROYAL CİTY</t>
-  </si>
-  <si>
     <t>Blok Adı*</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>AD1</t>
+    <t>Hakan Altun</t>
+  </si>
+  <si>
+    <t>Kat Maliki</t>
+  </si>
+  <si>
+    <t>Mülk Tipi*</t>
+  </si>
+  <si>
+    <t>Daire No*</t>
+  </si>
+  <si>
+    <t>Konut</t>
   </si>
   <si>
     <t>3+1</t>
   </si>
   <si>
-    <t>Hakan Altun</t>
-  </si>
-  <si>
-    <t>Kat Maliki</t>
-  </si>
-  <si>
-    <t>Mülk Tipi*</t>
-  </si>
-  <si>
-    <t>Konut</t>
+    <t>Erkek</t>
+  </si>
+  <si>
+    <t>Angora</t>
+  </si>
+  <si>
+    <t>A1-D1</t>
   </si>
 </sst>
 </file>
@@ -288,10 +294,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,31 +585,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,90 +621,113 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2">
+        <v>5551111111</v>
+      </c>
+      <c r="J2" s="2">
+        <v>45689</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2">
-        <v>5551111111</v>
-      </c>
-      <c r="I2" s="2">
-        <v>45658</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N251" xr:uid="{B5F827C4-9431-4AFB-A6DC-DDF6EEDE4799}">
+      <formula1>"Kat Maliki,Kiracı"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M250" xr:uid="{69991169-67F7-4FC7-900B-0F7C1B928FBF}">
+      <formula1>"Erkek,Kadın"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G250" xr:uid="{FC9AB616-09C9-4BEF-B20F-E2829E701B1C}">
+      <formula1>"3+1,2+1,1+1,İşyeri,Mağaza"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{68E0D79C-DB03-4511-AAA2-6C250E6B0A65}">
+      <formula1>"Konut,İşyeri,Depo,Otopark,Diğer"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>